<commit_message>
i am practicing git again
</commit_message>
<xml_diff>
--- a/TestData/Book1.xlsx
+++ b/TestData/Book1.xlsx
@@ -1382,7 +1382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
@@ -1414,89 +1414,173 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Kerala</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Tamil Nadu</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Andhra Pradesh</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>West Bengal</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Gujarat</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>Jammu and Kashmir</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>Himachal Pradesh</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>2</t>
         </is>

</xml_diff>